<commit_message>
Added Unit Tests for Parsing Time
</commit_message>
<xml_diff>
--- a/docs/testPlan.xlsx
+++ b/docs/testPlan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="19020" windowHeight="8580"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
   <si>
     <t>Test ID</t>
   </si>
@@ -196,13 +196,91 @@
   </si>
   <si>
     <t>Precondition: app is trying to add an event with endDay &gt; 29 when endMonth = 10</t>
+  </si>
+  <si>
+    <t>parseTimeForHour</t>
+  </si>
+  <si>
+    <t>Return 11</t>
+  </si>
+  <si>
+    <t>Return 13</t>
+  </si>
+  <si>
+    <t>Return 23</t>
+  </si>
+  <si>
+    <t>Return -1</t>
+  </si>
+  <si>
+    <t>Input Random String</t>
+  </si>
+  <si>
+    <t>Return 1</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "11:30am"</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "11:30pm"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "111:30am"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "111:30pm"</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "1:30am"</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "1:30pm"</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "01:30am"</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "01:30pm"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = ":30pm"</t>
+  </si>
+  <si>
+    <t>Return 30</t>
+  </si>
+  <si>
+    <t>Valid Input Test Case. Input = "11:26am"</t>
+  </si>
+  <si>
+    <t>Return 26</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "11:300am"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "11:am"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "11:0am"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "11:3am"</t>
+  </si>
+  <si>
+    <t>parseTimeForMinute</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "11:30"</t>
+  </si>
+  <si>
+    <t>Invalid Input Test Case. Input = "1130pm"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -352,6 +430,32 @@
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -368,7 +472,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,6 +505,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -410,6 +526,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -488,6 +609,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -522,6 +644,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -697,14 +820,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
@@ -712,7 +835,7 @@
     <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -734,7 +857,7 @@
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="1:4" ht="60.75" thickBot="1">
+    <row r="3" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -746,7 +869,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="60.75" thickBot="1">
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <f>A3+1</f>
         <v>2</v>
@@ -759,7 +882,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -767,7 +890,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="60.75" thickBot="1">
+    <row r="6" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -779,7 +902,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="60.75" thickBot="1">
+    <row r="7" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f>A6+1</f>
         <v>2</v>
@@ -792,7 +915,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -800,7 +923,7 @@
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
     </row>
-    <row r="9" spans="1:4" ht="60.75" thickBot="1">
+    <row r="9" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -812,7 +935,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="45.75" thickBot="1">
+    <row r="10" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <f>A9+1</f>
         <v>2</v>
@@ -825,7 +948,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="45.75" thickBot="1">
+    <row r="11" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <f t="shared" ref="A11:A53" si="0">A10+1</f>
         <v>3</v>
@@ -838,7 +961,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="60.75" thickBot="1">
+    <row r="12" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -851,7 +974,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" ht="60.75" thickBot="1">
+    <row r="13" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -864,7 +987,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" ht="45.75" thickBot="1">
+    <row r="14" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -877,7 +1000,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="45.75" thickBot="1">
+    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -890,7 +1013,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="45.75" thickBot="1">
+    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -903,7 +1026,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="45.75" thickBot="1">
+    <row r="17" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -916,7 +1039,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="75.75" thickBot="1">
+    <row r="18" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -929,7 +1052,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="75.75" thickBot="1">
+    <row r="19" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -942,7 +1065,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="45.75" thickBot="1">
+    <row r="20" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -955,7 +1078,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="45.75" thickBot="1">
+    <row r="21" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -968,7 +1091,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" ht="120.75" thickBot="1">
+    <row r="22" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -981,7 +1104,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="120.75" thickBot="1">
+    <row r="23" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -994,7 +1117,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" ht="120.75" thickBot="1">
+    <row r="24" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1007,7 +1130,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="120.75" thickBot="1">
+    <row r="25" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1020,7 +1143,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="60.75" thickBot="1">
+    <row r="26" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1033,7 +1156,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="60.75" thickBot="1">
+    <row r="27" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1046,7 +1169,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" ht="60.75" thickBot="1">
+    <row r="28" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1059,7 +1182,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="60.75" thickBot="1">
+    <row r="29" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1072,7 +1195,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="60.75" thickBot="1">
+    <row r="30" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1085,7 +1208,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="60.75" thickBot="1">
+    <row r="31" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1098,7 +1221,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" ht="60.75" thickBot="1">
+    <row r="32" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1111,7 +1234,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="60.75" thickBot="1">
+    <row r="33" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1124,7 +1247,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="45.75" thickBot="1">
+    <row r="34" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1137,7 +1260,7 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="45.75" thickBot="1">
+    <row r="35" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1150,7 +1273,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="90.75" thickBot="1">
+    <row r="36" spans="1:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1163,7 +1286,7 @@
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="90.75" thickBot="1">
+    <row r="37" spans="1:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1176,7 +1299,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="45.75" thickBot="1">
+    <row r="38" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1189,7 +1312,7 @@
       </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" ht="45.75" thickBot="1">
+    <row r="39" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1202,7 +1325,7 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" ht="45.75" thickBot="1">
+    <row r="40" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1215,7 +1338,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" ht="45.75" thickBot="1">
+    <row r="41" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1228,7 +1351,7 @@
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="105.75" thickBot="1">
+    <row r="42" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1241,7 +1364,7 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="105.75" thickBot="1">
+    <row r="43" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1254,7 +1377,7 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="45.75" thickBot="1">
+    <row r="44" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1267,7 +1390,7 @@
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="45.75" thickBot="1">
+    <row r="45" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1280,7 +1403,7 @@
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="45.75" thickBot="1">
+    <row r="46" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1293,7 +1416,7 @@
       </c>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="45.75" thickBot="1">
+    <row r="47" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1306,7 +1429,7 @@
       </c>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" ht="135.75" thickBot="1">
+    <row r="48" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1319,7 +1442,7 @@
       </c>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" ht="135.75" thickBot="1">
+    <row r="49" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1332,7 +1455,7 @@
       </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" ht="60.75" thickBot="1">
+    <row r="50" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1345,7 +1468,7 @@
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" ht="45.75" thickBot="1">
+    <row r="51" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1358,7 +1481,7 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" ht="60.75" thickBot="1">
+    <row r="52" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1371,7 +1494,7 @@
       </c>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" ht="45.75" thickBot="1">
+    <row r="53" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1384,11 +1507,279 @@
       </c>
       <c r="D53" s="6"/>
     </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
+    </row>
+    <row r="55" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="17">
+        <v>1</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <f>A55+1</f>
+        <v>2</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <f t="shared" ref="A57:A63" si="1">A56+1</f>
+        <v>3</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <f>A63+1</f>
+        <v>10</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <f>A64+1</f>
+        <v>11</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+    </row>
+    <row r="67" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="17">
+        <v>1</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <f>A67+1</f>
+        <v>2</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <f t="shared" ref="A69:A72" si="2">A68+1</f>
+        <v>3</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D71" s="20"/>
+    </row>
+    <row r="72" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <f t="shared" ref="A73" si="3">A72+1</f>
+        <v>7</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1396,24 +1787,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>